<commit_message>
re upload with brake energy and oei climb
</commit_message>
<xml_diff>
--- a/Q400 MELCDL Test Cases.xlsx
+++ b/Q400 MELCDL Test Cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\PycharmProjects\testing_validation_400_MELCDL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B8786F-D8F7-4441-9DDD-08032FC1E079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16BF39A-A274-4C08-8752-DD268ADD1533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C2D85D52-38C1-4259-BD73-DACB0394F242}"/>
   </bookViews>
@@ -22,14 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -61,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="59">
   <si>
     <t>Test Case Number</t>
   </si>
@@ -223,9 +215,6 @@
     <t>01</t>
   </si>
   <si>
-    <t>Changes made on 27/09/2023</t>
-  </si>
-  <si>
     <t>MELCDL</t>
   </si>
   <si>
@@ -242,9 +231,6 @@
   </si>
   <si>
     <t>INOP2 (FS)</t>
-  </si>
-  <si>
-    <t>Changes made on 29/08/2023</t>
   </si>
 </sst>
 </file>
@@ -824,9 +810,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C794B684-2E47-4CE0-843E-A8A5305D4DD9}">
   <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -928,7 +914,7 @@
         <v>19</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V1" s="11" t="s">
         <v>20</v>
@@ -1029,7 +1015,7 @@
         <v>34</v>
       </c>
       <c r="U2" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
@@ -1106,7 +1092,7 @@
         <v>34</v>
       </c>
       <c r="U3" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
@@ -1183,7 +1169,7 @@
         <v>34</v>
       </c>
       <c r="U4" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
@@ -1260,7 +1246,7 @@
         <v>34</v>
       </c>
       <c r="U5" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
@@ -1337,7 +1323,7 @@
         <v>34</v>
       </c>
       <c r="U6" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
@@ -1414,7 +1400,7 @@
         <v>39</v>
       </c>
       <c r="U7" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
@@ -1491,7 +1477,7 @@
         <v>34</v>
       </c>
       <c r="U8" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
@@ -1568,7 +1554,7 @@
         <v>34</v>
       </c>
       <c r="U9" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V9" s="12"/>
       <c r="W9" s="12"/>
@@ -1645,7 +1631,7 @@
         <v>34</v>
       </c>
       <c r="U10" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V10" s="12"/>
       <c r="W10" s="12"/>
@@ -1722,7 +1708,7 @@
         <v>39</v>
       </c>
       <c r="U11" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V11" s="12"/>
       <c r="W11" s="12"/>
@@ -1799,7 +1785,7 @@
         <v>34</v>
       </c>
       <c r="U12" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V12" s="12"/>
       <c r="W12" s="12"/>
@@ -1876,7 +1862,7 @@
         <v>34</v>
       </c>
       <c r="U13" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V13" s="12"/>
       <c r="W13" s="12"/>
@@ -1953,7 +1939,7 @@
         <v>39</v>
       </c>
       <c r="U14" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V14" s="12"/>
       <c r="W14" s="12"/>
@@ -2030,7 +2016,7 @@
         <v>39</v>
       </c>
       <c r="U15" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V15" s="12"/>
       <c r="W15" s="12"/>
@@ -2107,7 +2093,7 @@
         <v>34</v>
       </c>
       <c r="U16" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V16" s="12"/>
       <c r="W16" s="12"/>
@@ -2184,7 +2170,7 @@
         <v>39</v>
       </c>
       <c r="U17" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
@@ -2261,7 +2247,7 @@
         <v>34</v>
       </c>
       <c r="U18" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
@@ -2338,7 +2324,7 @@
         <v>39</v>
       </c>
       <c r="U19" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
@@ -2415,7 +2401,7 @@
         <v>34</v>
       </c>
       <c r="U20" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
@@ -2492,7 +2478,7 @@
         <v>39</v>
       </c>
       <c r="U21" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V21" s="12"/>
       <c r="W21" s="12"/>
@@ -2509,15 +2495,9 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A24" s="28"/>
-      <c r="B24" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A25" s="17"/>
-      <c r="B25" t="s">
-        <v>60</v>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG21" xr:uid="{5E53FA5F-CF5F-433A-A2DA-1F161F421E19}"/>
@@ -2538,23 +2518,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d78e05a7-6d5b-4941-b454-be5a632ec503" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095B7A33CA76A8846BF3FBE8249ED0F12" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff9261941b86076f8498d85a9bdcc20f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d78e05a7-6d5b-4941-b454-be5a632ec503" xmlns:ns4="f6a73a6d-4349-46c0-a653-75b157bab33f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e584b197f76ab1c18fef1086b16ccddf" ns3:_="" ns4:_="">
     <xsd:import namespace="d78e05a7-6d5b-4941-b454-be5a632ec503"/>
@@ -2787,25 +2750,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F19572-1A0E-4668-AD36-CDC9C822A928}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d78e05a7-6d5b-4941-b454-be5a632ec503" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD7A6922-8D8C-412B-A050-C578A4489D79}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d78e05a7-6d5b-4941-b454-be5a632ec503"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39522160-BD5D-4863-90DB-CFEB7E27C993}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2822,4 +2784,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD7A6922-8D8C-412B-A050-C578A4489D79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d78e05a7-6d5b-4941-b454-be5a632ec503"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F19572-1A0E-4668-AD36-CDC9C822A928}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>